<commit_message>
07062022 patrick : add field to mf and sf report, finance api update, finance import update
</commit_message>
<xml_diff>
--- a/files/finance_template.xlsx
+++ b/files/finance_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\patrick\Odesii\Doc\web project\ecob portal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\patrick\Odesii\Doc\API\odesi_skep\updated finance\API doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3F15E-C207-4515-96CD-206937C4968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="653" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
     <sheet name="Staff" sheetId="8" r:id="rId9"/>
     <sheet name="Admin" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
   <si>
     <t>CHECK DATE</t>
   </si>
@@ -384,16 +385,22 @@
   </si>
   <si>
     <t>scszcxccxx</t>
+  </si>
+  <si>
+    <t>TUNGGAKAN LAIN-LAIN</t>
+  </si>
+  <si>
+    <t>REPORT MF TUNGGAKAN BELUM DIKUTIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14409]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,11 +421,13 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Lato"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -795,14 +804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -860,7 +869,7 @@
     <col min="114" max="114" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -877,7 +886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>44120</v>
       </c>
@@ -900,14 +909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
@@ -916,7 +925,7 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -933,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>73</v>
       </c>
@@ -950,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>74</v>
       </c>
@@ -967,7 +976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>75</v>
       </c>
@@ -984,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
@@ -1001,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>77</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>78</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>79</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>80</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>81</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>82</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>83</v>
       </c>
@@ -1120,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>84</v>
       </c>
@@ -1137,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>85</v>
       </c>
@@ -1154,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -1171,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>87</v>
       </c>
@@ -1188,14 +1197,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1208,28 +1217,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1239,26 +1249,29 @@
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>700</v>
       </c>
@@ -1268,44 +1281,47 @@
       <c r="C2" s="8">
         <v>700</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
+        <v>10</v>
+      </c>
+      <c r="E2" s="9">
         <v>2342424324</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="F2" s="8">
-        <v>700</v>
       </c>
       <c r="G2" s="8">
         <v>700</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="H2" s="8">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
     </row>
@@ -1315,25 +1331,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1343,20 +1360,23 @@
       <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>700</v>
       </c>
@@ -1366,20 +1386,23 @@
       <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="8">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5">
         <v>12321312321</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="8">
+      <c r="G2" s="8">
         <v>20</v>
       </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1387,7 +1410,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1395,7 +1418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>21</v>
       </c>
@@ -1403,11 +1426,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
@@ -1418,21 +1441,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1446,7 +1469,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1460,7 +1483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1483,9 +1506,9 @@
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="5" t="s">
-        <v>25</v>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="B4" s="12">
         <v>10</v>
@@ -1496,10 +1519,19 @@
       <c r="D4" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="12">
         <v>10</v>
@@ -1511,9 +1543,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="12">
         <v>10</v>
@@ -1525,9 +1557,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="12">
         <v>10</v>
@@ -1539,9 +1571,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="12">
         <v>10</v>
@@ -1553,9 +1585,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="12">
         <v>10</v>
@@ -1567,9 +1599,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="12">
         <v>10</v>
@@ -1581,9 +1613,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="12">
         <v>10</v>
@@ -1595,9 +1627,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="12">
         <v>10</v>
@@ -1609,31 +1641,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="17" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B14" s="21">
         <v>10</v>
       </c>
-      <c r="C13" s="21">
-        <v>1</v>
-      </c>
-      <c r="D13" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="19"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="3"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="C14" s="21">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1641,14 +1687,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1657,7 +1703,7 @@
     <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
@@ -1673,7 +1719,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -1706,7 +1752,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>42</v>
       </c>
@@ -1738,7 +1784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>43</v>
       </c>
@@ -1770,21 +1816,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G5" s="19"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G6" s="3"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F9" s="2"/>
     </row>
   </sheetData>
@@ -1794,14 +1840,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1810,7 +1856,7 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -1837,7 +1883,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>46</v>
       </c>
@@ -1854,7 +1900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>47</v>
       </c>
@@ -1871,7 +1917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>48</v>
       </c>
@@ -1888,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>49</v>
       </c>
@@ -1905,7 +1951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>50</v>
       </c>
@@ -1922,7 +1968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -1939,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>52</v>
       </c>
@@ -1956,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
@@ -1973,7 +2019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
@@ -1990,7 +2036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -2007,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>56</v>
       </c>
@@ -2024,7 +2070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -2041,7 +2087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
@@ -2058,7 +2104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
@@ -2075,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>60</v>
       </c>
@@ -2092,14 +2138,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2112,14 +2158,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -2128,7 +2174,7 @@
     <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>88</v>
       </c>
@@ -2171,7 +2217,7 @@
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -2204,7 +2250,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -2236,7 +2282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>90</v>
       </c>
@@ -2268,7 +2314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>91</v>
       </c>
@@ -2300,7 +2346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>92</v>
       </c>
@@ -2332,7 +2378,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>93</v>
       </c>
@@ -2364,7 +2410,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>94</v>
       </c>
@@ -2396,7 +2442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>95</v>
       </c>
@@ -2428,7 +2474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>96</v>
       </c>
@@ -2460,7 +2506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>97</v>
       </c>
@@ -2492,7 +2538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>98</v>
       </c>
@@ -2524,7 +2570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>99</v>
       </c>
@@ -2556,7 +2602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>100</v>
       </c>
@@ -2588,7 +2634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>101</v>
       </c>
@@ -2620,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>102</v>
       </c>
@@ -2652,7 +2698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>103</v>
       </c>
@@ -2684,7 +2730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
@@ -2716,7 +2762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>104</v>
       </c>
@@ -2748,7 +2794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
@@ -2780,7 +2826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>105</v>
       </c>
@@ -2802,7 +2848,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -2814,7 +2860,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2827,14 +2873,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="G12" sqref="G12:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -2844,7 +2890,7 @@
     <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>88</v>
       </c>
@@ -2868,7 +2914,7 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
@@ -2901,7 +2947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -2933,7 +2979,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>96</v>
       </c>
@@ -2965,7 +3011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>97</v>
       </c>
@@ -2997,7 +3043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>100</v>
       </c>
@@ -3029,7 +3075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>102</v>
       </c>
@@ -3061,7 +3107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>106</v>
       </c>
@@ -3093,7 +3139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -3125,7 +3171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>104</v>
       </c>
@@ -3157,7 +3203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>105</v>
       </c>
@@ -3189,7 +3235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -3201,7 +3247,7 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -3219,14 +3265,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -3237,7 +3283,7 @@
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
@@ -3261,7 +3307,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>66</v>
       </c>
@@ -3284,7 +3330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
@@ -3307,7 +3353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>68</v>
       </c>
@@ -3330,7 +3376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
@@ -3353,7 +3399,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
@@ -3376,7 +3422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>71</v>
       </c>
@@ -3399,7 +3445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="26"/>
@@ -3408,7 +3454,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="16"/>
       <c r="C9" s="25"/>

</xml_diff>

<commit_message>
:zap: 28062022 patrick : finance utility add more button bhg A
</commit_message>
<xml_diff>
--- a/files/finance_template.xlsx
+++ b/files/finance_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\patrick\Odesii\Doc\API\odesi_skep\updated finance\API doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3F15E-C207-4515-96CD-206937C4968F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +18,7 @@
     <sheet name="Staff" sheetId="8" r:id="rId9"/>
     <sheet name="Admin" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
   <si>
     <t>CHECK DATE</t>
   </si>
@@ -88,9 +82,6 @@
   </si>
   <si>
     <t>REPORT SF BAKI BANK AKHIR</t>
-  </si>
-  <si>
-    <t>PERKARA</t>
   </si>
   <si>
     <t>JUMLAH</t>
@@ -396,11 +387,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14409]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,7 +576,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -620,7 +611,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,21 +788,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -869,7 +860,7 @@
     <col min="114" max="114" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -886,21 +877,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="14">
         <v>44120</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -909,14 +900,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
@@ -925,128 +916,128 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>64</v>
-      </c>
       <c r="D1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>2</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="8">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="8">
-        <v>4</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="8">
-        <v>5</v>
-      </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B7" s="8">
-        <v>6</v>
-      </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>2</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="B8" s="8">
         <v>7</v>
@@ -1061,9 +1052,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="8">
         <v>8</v>
@@ -1078,9 +1069,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="8">
         <v>9</v>
@@ -1095,9 +1086,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="8">
         <v>10</v>
@@ -1112,9 +1103,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="8">
         <v>11</v>
@@ -1129,9 +1120,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="8">
         <v>12</v>
@@ -1146,9 +1137,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="8">
         <v>13</v>
@@ -1163,9 +1154,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8">
         <v>14</v>
@@ -1180,9 +1171,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="18">
         <v>15</v>
@@ -1197,14 +1188,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1217,14 +1208,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
@@ -1239,7 +1230,7 @@
     <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>8</v>
@@ -1271,7 +1262,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" s="8">
         <v>700</v>
       </c>
@@ -1288,7 +1279,7 @@
         <v>2342424324</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="8">
         <v>700</v>
@@ -1297,31 +1288,31 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
     </row>
@@ -1331,14 +1322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1350,7 +1341,7 @@
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1361,10 +1352,10 @@
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>15</v>
@@ -1376,7 +1367,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="8">
         <v>700</v>
       </c>
@@ -1393,7 +1384,7 @@
         <v>12321312321</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="8">
         <v>20</v>
@@ -1402,35 +1393,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B10" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="18">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
@@ -1441,37 +1432,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="B2" s="12">
         <v>10</v>
@@ -1483,9 +1474,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="12">
         <v>10</v>
@@ -1506,9 +1497,9 @@
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="12">
         <v>10</v>
@@ -1529,9 +1520,9 @@
       <c r="L4" s="1"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="12">
         <v>10</v>
@@ -1543,9 +1534,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="12">
         <v>10</v>
@@ -1557,9 +1548,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="12">
         <v>10</v>
@@ -1571,9 +1562,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="12">
         <v>10</v>
@@ -1585,9 +1576,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="12">
         <v>10</v>
@@ -1599,9 +1590,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="12">
         <v>10</v>
@@ -1613,9 +1604,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="12">
         <v>10</v>
@@ -1627,9 +1618,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="12">
         <v>10</v>
@@ -1641,9 +1632,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="12">
         <v>10</v>
@@ -1655,9 +1646,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="21">
         <v>10</v>
@@ -1669,13 +1660,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="19"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="3"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -1687,75 +1678,75 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="5"/>
       <c r="G1" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="B3" s="8">
         <v>1</v>
       </c>
@@ -1769,7 +1760,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1784,25 +1775,25 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>4</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>44</v>
-      </c>
       <c r="H4" s="18">
         <v>1</v>
       </c>
@@ -1816,21 +1807,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="G5" s="19"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="G6" s="3"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="F9" s="2"/>
     </row>
   </sheetData>
@@ -1840,14 +1831,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1856,21 +1847,21 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1883,248 +1874,248 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8">
+        <v>3</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="8">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8">
-        <v>3</v>
-      </c>
-      <c r="E3" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8">
-        <v>3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="8">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="8">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8">
-        <v>3</v>
-      </c>
-      <c r="E6" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="8">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8">
-        <v>3</v>
-      </c>
-      <c r="D7" s="8">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>3</v>
-      </c>
-      <c r="E8" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="8">
+        <v>3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="8">
-        <v>3</v>
-      </c>
-      <c r="C9" s="8">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8">
-        <v>3</v>
-      </c>
-      <c r="E9" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="8">
-        <v>3</v>
-      </c>
-      <c r="C10" s="8">
-        <v>3</v>
-      </c>
-      <c r="D10" s="8">
-        <v>3</v>
-      </c>
-      <c r="E10" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="8">
+        <v>3</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="8">
-        <v>3</v>
-      </c>
-      <c r="C11" s="8">
-        <v>3</v>
-      </c>
-      <c r="D11" s="8">
-        <v>3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="8">
+        <v>3</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="8">
-        <v>3</v>
-      </c>
-      <c r="C12" s="8">
-        <v>3</v>
-      </c>
-      <c r="D12" s="8">
-        <v>3</v>
-      </c>
-      <c r="E12" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="8">
-        <v>3</v>
-      </c>
-      <c r="C13" s="8">
-        <v>3</v>
-      </c>
-      <c r="D13" s="8">
-        <v>3</v>
-      </c>
-      <c r="E13" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="8">
-        <v>3</v>
-      </c>
-      <c r="C14" s="8">
-        <v>3</v>
-      </c>
-      <c r="D14" s="8">
-        <v>3</v>
-      </c>
-      <c r="E14" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="8">
-        <v>3</v>
-      </c>
-      <c r="C15" s="8">
-        <v>3</v>
-      </c>
-      <c r="D15" s="8">
-        <v>3</v>
-      </c>
-      <c r="E15" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>60</v>
-      </c>
       <c r="B16" s="18">
         <v>2</v>
       </c>
@@ -2138,14 +2129,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2158,14 +2149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -2174,9 +2165,9 @@
     <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2184,7 +2175,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -2217,601 +2208,601 @@
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="8">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4</v>
+      </c>
+      <c r="I3" s="8">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8">
+        <v>4</v>
+      </c>
+      <c r="K3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="8">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8">
-        <v>4</v>
-      </c>
-      <c r="D3" s="8">
-        <v>4</v>
-      </c>
-      <c r="E3" s="8">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="B4" s="8">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="8">
-        <v>4</v>
-      </c>
-      <c r="I3" s="8">
-        <v>4</v>
-      </c>
-      <c r="J3" s="8">
-        <v>4</v>
-      </c>
-      <c r="K3" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="H4" s="8">
+        <v>4</v>
+      </c>
+      <c r="I4" s="8">
+        <v>4</v>
+      </c>
+      <c r="J4" s="8">
+        <v>4</v>
+      </c>
+      <c r="K4" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="8">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
-        <v>4</v>
-      </c>
-      <c r="E4" s="8">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="8">
-        <v>4</v>
-      </c>
-      <c r="I4" s="8">
-        <v>4</v>
-      </c>
-      <c r="J4" s="8">
-        <v>4</v>
-      </c>
-      <c r="K4" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="H5" s="8">
+        <v>4</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4</v>
+      </c>
+      <c r="J5" s="8">
+        <v>4</v>
+      </c>
+      <c r="K5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37">
+      <c r="A6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="8">
-        <v>4</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="8">
-        <v>4</v>
-      </c>
-      <c r="I5" s="8">
-        <v>4</v>
-      </c>
-      <c r="J5" s="8">
-        <v>4</v>
-      </c>
-      <c r="K5" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="H6" s="8">
+        <v>4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>4</v>
+      </c>
+      <c r="J6" s="8">
+        <v>4</v>
+      </c>
+      <c r="K6" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37">
+      <c r="A7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>4</v>
-      </c>
-      <c r="E6" s="8">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="B7" s="8">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="8">
-        <v>4</v>
-      </c>
-      <c r="I6" s="8">
-        <v>4</v>
-      </c>
-      <c r="J6" s="8">
-        <v>4</v>
-      </c>
-      <c r="K6" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="H7" s="8">
+        <v>4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4</v>
+      </c>
+      <c r="J7" s="8">
+        <v>4</v>
+      </c>
+      <c r="K7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="8">
-        <v>4</v>
-      </c>
-      <c r="C7" s="8">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8">
-        <v>4</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="8">
-        <v>4</v>
-      </c>
-      <c r="I7" s="8">
-        <v>4</v>
-      </c>
-      <c r="J7" s="8">
-        <v>4</v>
-      </c>
-      <c r="K7" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="H8" s="8">
+        <v>4</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="8">
+        <v>4</v>
+      </c>
+      <c r="K8" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37">
+      <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="8">
-        <v>4</v>
-      </c>
-      <c r="C8" s="8">
-        <v>4</v>
-      </c>
-      <c r="D8" s="8">
-        <v>4</v>
-      </c>
-      <c r="E8" s="8">
-        <v>4</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="B9" s="8">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="8">
-        <v>4</v>
-      </c>
-      <c r="I8" s="8">
-        <v>4</v>
-      </c>
-      <c r="J8" s="8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="H9" s="8">
+        <v>4</v>
+      </c>
+      <c r="I9" s="8">
+        <v>4</v>
+      </c>
+      <c r="J9" s="8">
+        <v>4</v>
+      </c>
+      <c r="K9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
+      <c r="A10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="8">
-        <v>4</v>
-      </c>
-      <c r="C9" s="8">
-        <v>4</v>
-      </c>
-      <c r="D9" s="8">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8">
-        <v>4</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="H9" s="8">
-        <v>4</v>
-      </c>
-      <c r="I9" s="8">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8">
-        <v>4</v>
-      </c>
-      <c r="K9" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="H10" s="8">
+        <v>4</v>
+      </c>
+      <c r="I10" s="8">
+        <v>4</v>
+      </c>
+      <c r="J10" s="8">
+        <v>4</v>
+      </c>
+      <c r="K10" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37">
+      <c r="A11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="8">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8">
-        <v>4</v>
-      </c>
-      <c r="D10" s="8">
-        <v>4</v>
-      </c>
-      <c r="E10" s="8">
-        <v>4</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="B11" s="8">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="8">
-        <v>4</v>
-      </c>
-      <c r="I10" s="8">
-        <v>4</v>
-      </c>
-      <c r="J10" s="8">
-        <v>4</v>
-      </c>
-      <c r="K10" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="H11" s="8">
+        <v>4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>4</v>
+      </c>
+      <c r="J11" s="8">
+        <v>4</v>
+      </c>
+      <c r="K11" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="8">
-        <v>4</v>
-      </c>
-      <c r="C11" s="8">
-        <v>4</v>
-      </c>
-      <c r="D11" s="8">
-        <v>4</v>
-      </c>
-      <c r="E11" s="8">
-        <v>4</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="B12" s="8">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="8">
-        <v>4</v>
-      </c>
-      <c r="I11" s="8">
-        <v>4</v>
-      </c>
-      <c r="J11" s="8">
-        <v>4</v>
-      </c>
-      <c r="K11" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="H12" s="8">
+        <v>4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>4</v>
+      </c>
+      <c r="J12" s="8">
+        <v>4</v>
+      </c>
+      <c r="K12" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="8">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8">
-        <v>4</v>
-      </c>
-      <c r="D12" s="8">
-        <v>4</v>
-      </c>
-      <c r="E12" s="8">
-        <v>4</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="B13" s="8">
+        <v>5</v>
+      </c>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="8">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H12" s="8">
-        <v>4</v>
-      </c>
-      <c r="I12" s="8">
-        <v>4</v>
-      </c>
-      <c r="J12" s="8">
-        <v>4</v>
-      </c>
-      <c r="K12" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="H13" s="8">
+        <v>5</v>
+      </c>
+      <c r="I13" s="8">
+        <v>5</v>
+      </c>
+      <c r="J13" s="8">
+        <v>6</v>
+      </c>
+      <c r="K13" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="8">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8">
-        <v>5</v>
-      </c>
-      <c r="D13" s="8">
-        <v>6</v>
-      </c>
-      <c r="E13" s="8">
-        <v>5</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="B14" s="8">
+        <v>5</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>6</v>
+      </c>
+      <c r="E14" s="8">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="8">
-        <v>5</v>
-      </c>
-      <c r="I13" s="8">
-        <v>5</v>
-      </c>
-      <c r="J13" s="8">
-        <v>6</v>
-      </c>
-      <c r="K13" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="H14" s="8">
+        <v>5</v>
+      </c>
+      <c r="I14" s="8">
+        <v>5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>6</v>
+      </c>
+      <c r="K14" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="8">
-        <v>5</v>
-      </c>
-      <c r="C14" s="8">
-        <v>5</v>
-      </c>
-      <c r="D14" s="8">
-        <v>6</v>
-      </c>
-      <c r="E14" s="8">
-        <v>5</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="B15" s="8">
+        <v>5</v>
+      </c>
+      <c r="C15" s="8">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8">
+        <v>6</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="8">
-        <v>5</v>
-      </c>
-      <c r="I14" s="8">
-        <v>5</v>
-      </c>
-      <c r="J14" s="8">
-        <v>6</v>
-      </c>
-      <c r="K14" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="H15" s="8">
+        <v>5</v>
+      </c>
+      <c r="I15" s="8">
+        <v>5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>6</v>
+      </c>
+      <c r="K15" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B15" s="8">
-        <v>5</v>
-      </c>
-      <c r="C15" s="8">
-        <v>5</v>
-      </c>
-      <c r="D15" s="8">
-        <v>6</v>
-      </c>
-      <c r="E15" s="8">
-        <v>5</v>
-      </c>
-      <c r="G15" s="5" t="s">
+      <c r="B16" s="8">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8">
+        <v>5</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="8">
-        <v>5</v>
-      </c>
-      <c r="I15" s="8">
-        <v>5</v>
-      </c>
-      <c r="J15" s="8">
-        <v>6</v>
-      </c>
-      <c r="K15" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="H16" s="8">
+        <v>5</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>6</v>
+      </c>
+      <c r="K16" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="8">
-        <v>5</v>
-      </c>
-      <c r="C16" s="8">
-        <v>5</v>
-      </c>
-      <c r="D16" s="8">
-        <v>6</v>
-      </c>
-      <c r="E16" s="8">
-        <v>5</v>
-      </c>
-      <c r="G16" s="5" t="s">
+      <c r="B17" s="8">
+        <v>5</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8">
+        <v>6</v>
+      </c>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H16" s="8">
-        <v>5</v>
-      </c>
-      <c r="I16" s="8">
-        <v>5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>6</v>
-      </c>
-      <c r="K16" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="H17" s="8">
+        <v>5</v>
+      </c>
+      <c r="I17" s="8">
+        <v>5</v>
+      </c>
+      <c r="J17" s="8">
+        <v>6</v>
+      </c>
+      <c r="K17" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="8">
+        <v>5</v>
+      </c>
+      <c r="C18" s="8">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="8">
+        <v>5</v>
+      </c>
+      <c r="I18" s="8">
+        <v>5</v>
+      </c>
+      <c r="J18" s="8">
+        <v>6</v>
+      </c>
+      <c r="K18" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B17" s="8">
-        <v>5</v>
-      </c>
-      <c r="C17" s="8">
-        <v>5</v>
-      </c>
-      <c r="D17" s="8">
-        <v>6</v>
-      </c>
-      <c r="E17" s="8">
-        <v>5</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="B19" s="8">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>5</v>
+      </c>
+      <c r="D19" s="8">
+        <v>6</v>
+      </c>
+      <c r="E19" s="8">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="8">
-        <v>5</v>
-      </c>
-      <c r="I17" s="8">
-        <v>5</v>
-      </c>
-      <c r="J17" s="8">
-        <v>6</v>
-      </c>
-      <c r="K17" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="8">
-        <v>5</v>
-      </c>
-      <c r="C18" s="8">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8">
-        <v>6</v>
-      </c>
-      <c r="E18" s="8">
-        <v>5</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="8">
-        <v>5</v>
-      </c>
-      <c r="I18" s="8">
-        <v>5</v>
-      </c>
-      <c r="J18" s="8">
-        <v>6</v>
-      </c>
-      <c r="K18" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="H19" s="8">
+        <v>5</v>
+      </c>
+      <c r="I19" s="8">
+        <v>5</v>
+      </c>
+      <c r="J19" s="8">
+        <v>6</v>
+      </c>
+      <c r="K19" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="8">
+        <v>5</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5</v>
+      </c>
+      <c r="D20" s="8">
+        <v>6</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="B19" s="8">
-        <v>5</v>
-      </c>
-      <c r="C19" s="8">
-        <v>5</v>
-      </c>
-      <c r="D19" s="8">
-        <v>6</v>
-      </c>
-      <c r="E19" s="8">
-        <v>5</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="8">
-        <v>5</v>
-      </c>
-      <c r="I19" s="8">
-        <v>5</v>
-      </c>
-      <c r="J19" s="8">
-        <v>6</v>
-      </c>
-      <c r="K19" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="8">
-        <v>5</v>
-      </c>
-      <c r="C20" s="8">
-        <v>5</v>
-      </c>
-      <c r="D20" s="8">
-        <v>6</v>
-      </c>
-      <c r="E20" s="8">
-        <v>5</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="H20" s="18">
         <v>7</v>
@@ -2826,9 +2817,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="18">
         <v>7</v>
@@ -2848,7 +2839,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -2860,7 +2851,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2873,14 +2864,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="G12" sqref="G12:K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -2890,9 +2881,9 @@
     <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2900,7 +2891,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -2914,42 +2905,42 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -2964,7 +2955,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -2979,57 +2970,57 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18">
       <c r="A4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>4</v>
+      </c>
+      <c r="J4" s="8">
+        <v>5</v>
+      </c>
+      <c r="K4" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H4" s="8">
-        <v>2</v>
-      </c>
-      <c r="I4" s="8">
-        <v>4</v>
-      </c>
-      <c r="J4" s="8">
-        <v>5</v>
-      </c>
-      <c r="K4" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>5</v>
-      </c>
-      <c r="E5" s="8">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="H5" s="8">
         <v>3</v>
       </c>
@@ -3043,9 +3034,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
@@ -3060,7 +3051,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -3075,9 +3066,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3092,7 +3083,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="8">
         <v>5</v>
@@ -3107,9 +3098,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3124,7 +3115,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -3139,9 +3130,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3156,7 +3147,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -3171,9 +3162,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3188,7 +3179,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -3203,9 +3194,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="18">
         <v>9</v>
@@ -3220,7 +3211,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H11" s="18">
         <v>9</v>
@@ -3235,7 +3226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -3247,7 +3238,7 @@
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -3265,14 +3256,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -3283,149 +3274,149 @@
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="8">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="8">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="8">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>71</v>
-      </c>
       <c r="B7" s="18">
         <v>6</v>
       </c>
@@ -3445,7 +3436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="26"/>
@@ -3454,7 +3445,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3"/>
       <c r="B9" s="16"/>
       <c r="C9" s="25"/>

</xml_diff>

<commit_message>
:sparkles: 21072022 patrick : add notification module, add notify & email to JMB every action and send to COB, MPS OB Letter Module, API Client & API Building Module, Finance API Updates
</commit_message>
<xml_diff>
--- a/files/finance_template.xlsx
+++ b/files/finance_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>CHECK DATE</t>
   </si>
@@ -39,9 +39,6 @@
     <t>CHECK POSITION</t>
   </si>
   <si>
-    <t>CHECK STATUS (YES/NO)</t>
-  </si>
-  <si>
     <t>REMARKS (IF HAVE)</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
   </si>
   <si>
     <t>test_position</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>kajsdakjsdkjasbd</t>
@@ -788,7 +782,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -796,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -807,60 +801,59 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="39" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="34" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="39" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="34" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -873,25 +866,19 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="14">
         <v>44120</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -918,24 +905,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
@@ -952,7 +939,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
@@ -969,7 +956,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
@@ -986,7 +973,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="8">
         <v>4</v>
@@ -1003,7 +990,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
@@ -1020,7 +1007,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="8">
         <v>6</v>
@@ -1037,7 +1024,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="8">
         <v>7</v>
@@ -1054,7 +1041,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="8">
         <v>8</v>
@@ -1071,7 +1058,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="8">
         <v>9</v>
@@ -1088,7 +1075,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="8">
         <v>10</v>
@@ -1105,7 +1092,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="8">
         <v>11</v>
@@ -1122,7 +1109,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="8">
         <v>12</v>
@@ -1139,7 +1126,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="8">
         <v>13</v>
@@ -1156,7 +1143,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="8">
         <v>14</v>
@@ -1173,7 +1160,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="18">
         <v>15</v>
@@ -1232,28 +1219,28 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1279,7 +1266,7 @@
         <v>2342424324</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="8">
         <v>700</v>
@@ -1343,28 +1330,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1384,7 +1371,7 @@
         <v>12321312321</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G2" s="8">
         <v>20</v>
@@ -1395,15 +1382,15 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="8">
         <v>10</v>
@@ -1411,7 +1398,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="18">
         <v>20</v>
@@ -1448,21 +1435,21 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="12">
         <v>10</v>
@@ -1476,7 +1463,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="12">
         <v>10</v>
@@ -1499,7 +1486,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="12">
         <v>10</v>
@@ -1522,7 +1509,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="12">
         <v>10</v>
@@ -1536,7 +1523,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="12">
         <v>10</v>
@@ -1550,7 +1537,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12">
         <v>10</v>
@@ -1564,7 +1551,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="12">
         <v>10</v>
@@ -1578,7 +1565,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="12">
         <v>10</v>
@@ -1592,7 +1579,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="12">
         <v>10</v>
@@ -1606,7 +1593,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="12">
         <v>10</v>
@@ -1620,7 +1607,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12">
         <v>10</v>
@@ -1634,7 +1621,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="12">
         <v>10</v>
@@ -1648,7 +1635,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="21">
         <v>10</v>
@@ -1681,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1696,14 +1683,14 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="5"/>
       <c r="G1" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -1712,40 +1699,40 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -1760,7 +1747,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -1777,22 +1764,22 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>4</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>43</v>
       </c>
       <c r="H4" s="18">
         <v>1</v>
@@ -1849,19 +1836,19 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1876,7 +1863,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="8">
         <v>3</v>
@@ -1893,7 +1880,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -1910,7 +1897,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
@@ -1927,7 +1914,7 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -1944,7 +1931,7 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="8">
         <v>3</v>
@@ -1961,7 +1948,7 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="8">
         <v>3</v>
@@ -1978,7 +1965,7 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="8">
         <v>3</v>
@@ -1995,7 +1982,7 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="8">
         <v>3</v>
@@ -2012,7 +1999,7 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="8">
         <v>3</v>
@@ -2029,7 +2016,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="8">
         <v>3</v>
@@ -2046,7 +2033,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="8">
         <v>3</v>
@@ -2063,7 +2050,7 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
@@ -2080,7 +2067,7 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="8">
         <v>3</v>
@@ -2097,7 +2084,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="8">
         <v>3</v>
@@ -2114,7 +2101,7 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="18">
         <v>2</v>
@@ -2167,7 +2154,7 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2175,7 +2162,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -2210,40 +2197,40 @@
     </row>
     <row r="2" spans="1:37">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8">
         <v>4</v>
@@ -2258,7 +2245,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H3" s="8">
         <v>4</v>
@@ -2275,7 +2262,7 @@
     </row>
     <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="8">
         <v>4</v>
@@ -2290,7 +2277,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="8">
         <v>4</v>
@@ -2307,7 +2294,7 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="8">
         <v>4</v>
@@ -2322,7 +2309,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" s="8">
         <v>4</v>
@@ -2339,7 +2326,7 @@
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
@@ -2354,7 +2341,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -2371,7 +2358,7 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="8">
         <v>4</v>
@@ -2386,7 +2373,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="8">
         <v>4</v>
@@ -2403,7 +2390,7 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B8" s="8">
         <v>4</v>
@@ -2418,7 +2405,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="8">
         <v>4</v>
@@ -2435,7 +2422,7 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B9" s="8">
         <v>4</v>
@@ -2450,7 +2437,7 @@
         <v>4</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" s="8">
         <v>4</v>
@@ -2467,7 +2454,7 @@
     </row>
     <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="8">
         <v>4</v>
@@ -2482,7 +2469,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H10" s="8">
         <v>4</v>
@@ -2499,7 +2486,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="8">
         <v>4</v>
@@ -2514,7 +2501,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="8">
         <v>4</v>
@@ -2531,7 +2518,7 @@
     </row>
     <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="8">
         <v>4</v>
@@ -2546,7 +2533,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H12" s="8">
         <v>4</v>
@@ -2563,7 +2550,7 @@
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B13" s="8">
         <v>5</v>
@@ -2578,7 +2565,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H13" s="8">
         <v>5</v>
@@ -2595,7 +2582,7 @@
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="8">
         <v>5</v>
@@ -2610,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H14" s="8">
         <v>5</v>
@@ -2627,7 +2614,7 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="8">
         <v>5</v>
@@ -2642,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H15" s="8">
         <v>5</v>
@@ -2659,7 +2646,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="8">
         <v>5</v>
@@ -2674,7 +2661,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H16" s="8">
         <v>5</v>
@@ -2691,7 +2678,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B17" s="8">
         <v>5</v>
@@ -2706,7 +2693,7 @@
         <v>5</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" s="8">
         <v>5</v>
@@ -2723,7 +2710,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="8">
         <v>5</v>
@@ -2738,7 +2725,7 @@
         <v>5</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H18" s="8">
         <v>5</v>
@@ -2755,7 +2742,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="8">
         <v>5</v>
@@ -2770,7 +2757,7 @@
         <v>5</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="8">
         <v>5</v>
@@ -2787,7 +2774,7 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="8">
         <v>5</v>
@@ -2802,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" s="18">
         <v>7</v>
@@ -2819,7 +2806,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="18">
         <v>7</v>
@@ -2883,7 +2870,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2891,7 +2878,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="1"/>
       <c r="G1" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -2907,40 +2894,40 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="8">
         <v>1</v>
@@ -2955,7 +2942,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H3" s="8">
         <v>1</v>
@@ -2972,7 +2959,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="8">
         <v>2</v>
@@ -2987,7 +2974,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" s="8">
         <v>2</v>
@@ -3004,7 +2991,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="8">
         <v>3</v>
@@ -3019,7 +3006,7 @@
         <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H5" s="8">
         <v>3</v>
@@ -3036,7 +3023,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="8">
         <v>4</v>
@@ -3051,7 +3038,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="8">
         <v>4</v>
@@ -3068,7 +3055,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="8">
         <v>5</v>
@@ -3083,7 +3070,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="8">
         <v>5</v>
@@ -3100,7 +3087,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="8">
         <v>6</v>
@@ -3115,7 +3102,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H8" s="8">
         <v>6</v>
@@ -3132,7 +3119,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="8">
         <v>7</v>
@@ -3147,7 +3134,7 @@
         <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" s="8">
         <v>7</v>
@@ -3164,7 +3151,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="8">
         <v>8</v>
@@ -3179,7 +3166,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H10" s="8">
         <v>8</v>
@@ -3196,7 +3183,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="18">
         <v>9</v>
@@ -3211,7 +3198,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="18">
         <v>9</v>
@@ -3276,31 +3263,31 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
@@ -3323,7 +3310,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="8">
         <v>2</v>
@@ -3346,7 +3333,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="8">
         <v>3</v>
@@ -3369,7 +3356,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" s="8">
         <v>4</v>
@@ -3392,7 +3379,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
@@ -3415,7 +3402,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="18">
         <v>6</v>

</xml_diff>

<commit_message>
Bugs fix & enhancements
</commit_message>
<xml_diff>
--- a/files/finance_template.xlsx
+++ b/files/finance_template.xlsx
@@ -1,34 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\skep\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031A066-36E1-4DD3-B43A-BEA3F96553ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="653"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" tabRatio="653" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Report MF" sheetId="2" r:id="rId2"/>
-    <sheet name="Report SF" sheetId="10" r:id="rId3"/>
-    <sheet name="Income" sheetId="3" r:id="rId4"/>
-    <sheet name="Utility" sheetId="4" r:id="rId5"/>
-    <sheet name="Contract" sheetId="5" r:id="rId6"/>
-    <sheet name="Repair" sheetId="6" r:id="rId7"/>
-    <sheet name="Vandalisme" sheetId="7" r:id="rId8"/>
-    <sheet name="Staff" sheetId="8" r:id="rId9"/>
-    <sheet name="Admin" sheetId="9" r:id="rId10"/>
+    <sheet name="Report MF Additional" sheetId="11" r:id="rId3"/>
+    <sheet name="Report SF" sheetId="10" r:id="rId4"/>
+    <sheet name="Report SF Additional" sheetId="12" r:id="rId5"/>
+    <sheet name="Income" sheetId="3" r:id="rId6"/>
+    <sheet name="Utility" sheetId="4" r:id="rId7"/>
+    <sheet name="Contract" sheetId="5" r:id="rId8"/>
+    <sheet name="Repair" sheetId="6" r:id="rId9"/>
+    <sheet name="Vandalisme" sheetId="7" r:id="rId10"/>
+    <sheet name="Staff" sheetId="8" r:id="rId11"/>
+    <sheet name="Admin" sheetId="9" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
   <si>
     <t>CHECK DATE</t>
   </si>
@@ -357,35 +376,32 @@
     <t>SEMASA A</t>
   </si>
   <si>
-    <t>asdasdasdads</t>
-  </si>
-  <si>
     <t>test2</t>
   </si>
   <si>
     <t>test_position</t>
   </si>
   <si>
-    <t>kajsdakjsdkjasbd</t>
-  </si>
-  <si>
-    <t>scszcxccxx</t>
-  </si>
-  <si>
     <t>TUNGGAKAN LAIN-LAIN</t>
   </si>
   <si>
     <t>REPORT MF TUNGGAKAN BELUM DIKUTIP</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>REPORT SF TUNGGAKAN BELUM DIKUTIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14409]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,6 +526,21 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,78 +813,78 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="23" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.109375" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="39" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="53.88671875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="34" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -867,19 +898,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>44120</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>112</v>
-      </c>
+      <c r="D2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,23 +916,619 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:R13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>4</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8">
+        <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8">
+        <v>5</v>
+      </c>
+      <c r="K3" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8">
+        <v>4</v>
+      </c>
+      <c r="J4" s="8">
+        <v>5</v>
+      </c>
+      <c r="K4" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4</v>
+      </c>
+      <c r="J5" s="8">
+        <v>5</v>
+      </c>
+      <c r="K5" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>6</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="8">
+        <v>4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>4</v>
+      </c>
+      <c r="J6" s="8">
+        <v>5</v>
+      </c>
+      <c r="K6" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="8">
+        <v>5</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4</v>
+      </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5</v>
+      </c>
+      <c r="E8" s="8">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="8">
+        <v>6</v>
+      </c>
+      <c r="I8" s="8">
+        <v>4</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>5</v>
+      </c>
+      <c r="E9" s="8">
+        <v>6</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="8">
+        <v>7</v>
+      </c>
+      <c r="I9" s="8">
+        <v>4</v>
+      </c>
+      <c r="J9" s="8">
+        <v>5</v>
+      </c>
+      <c r="K9" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="8">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="8">
+        <v>8</v>
+      </c>
+      <c r="I10" s="8">
+        <v>4</v>
+      </c>
+      <c r="J10" s="8">
+        <v>5</v>
+      </c>
+      <c r="K10" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="18">
+        <v>9</v>
+      </c>
+      <c r="C11" s="18">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2</v>
+      </c>
+      <c r="E11" s="18">
+        <v>3</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="18">
+        <v>9</v>
+      </c>
+      <c r="I11" s="18">
+        <v>1</v>
+      </c>
+      <c r="J11" s="18">
+        <v>2</v>
+      </c>
+      <c r="K11" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>4</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="18">
+        <v>6</v>
+      </c>
+      <c r="C7" s="24">
+        <v>6</v>
+      </c>
+      <c r="D7" s="18">
+        <v>6</v>
+      </c>
+      <c r="E7" s="18">
+        <v>6</v>
+      </c>
+      <c r="F7" s="18">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -920,7 +1545,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
@@ -937,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>72</v>
       </c>
@@ -954,7 +1579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>73</v>
       </c>
@@ -971,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -988,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
@@ -1005,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
@@ -1022,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>77</v>
       </c>
@@ -1039,7 +1664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>78</v>
       </c>
@@ -1056,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -1073,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>80</v>
       </c>
@@ -1090,7 +1715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>81</v>
       </c>
@@ -1107,7 +1732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>82</v>
       </c>
@@ -1124,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -1141,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
@@ -1158,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>85</v>
       </c>
@@ -1175,14 +1800,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1195,29 +1820,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1228,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>7</v>
@@ -1249,14 +1874,15 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="8">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
         <v>700</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="27">
+        <f>SUM(A2 * B2)</f>
         <v>700</v>
       </c>
       <c r="D2" s="8">
@@ -1266,7 +1892,7 @@
         <v>2342424324</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G2" s="8">
         <v>700</v>
@@ -1275,31 +1901,31 @@
         <v>700</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
     </row>
@@ -1309,26 +1935,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6DBA9B-1E43-4ED0-A205-563C6E83F678}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>300</v>
+      </c>
+      <c r="B2" s="9">
+        <v>5</v>
+      </c>
+      <c r="C2" s="27">
+        <f>SUM(A2 * B2)</f>
+        <v>1500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -1339,7 +2009,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>105</v>
@@ -1354,15 +2024,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
         <v>700</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="9">
         <v>10</v>
       </c>
-      <c r="C2" s="8">
-        <v>2</v>
+      <c r="C2" s="27">
+        <f>SUM(A2 * B2)</f>
+        <v>7000</v>
       </c>
       <c r="D2" s="8">
         <v>10</v>
@@ -1380,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>20</v>
       </c>
@@ -1388,7 +2059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -1396,7 +2067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>19</v>
       </c>
@@ -1404,11 +2075,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
     </row>
@@ -1418,22 +2089,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AAB735B-97DD-4514-9F39-DD5DA2ECA110}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="64.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="27">
+        <v>200</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+      <c r="C2" s="27">
+        <f>SUM(A2 * B2)</f>
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1447,7 +2162,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -1461,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>22</v>
       </c>
@@ -1484,9 +2199,9 @@
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" s="12">
         <v>10</v>
@@ -1507,7 +2222,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
@@ -1521,7 +2236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +2250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
@@ -1549,7 +2264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
@@ -1563,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -1577,7 +2292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1591,7 +2306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
@@ -1605,7 +2320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
@@ -1619,7 +2334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
@@ -1633,7 +2348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>32</v>
       </c>
@@ -1647,13 +2362,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
@@ -1664,24 +2379,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1697,7 +2412,7 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -1730,7 +2445,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1762,7 +2477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
@@ -1794,21 +2509,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G5" s="19"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G6" s="3"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F9" s="2"/>
     </row>
   </sheetData>
@@ -1817,24 +2532,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1861,7 +2576,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>44</v>
       </c>
@@ -1878,7 +2593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
@@ -1895,7 +2610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>46</v>
       </c>
@@ -1912,7 +2627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -1929,7 +2644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>48</v>
       </c>
@@ -1946,7 +2661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>49</v>
       </c>
@@ -1963,7 +2678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -1980,7 +2695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -1997,7 +2712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -2014,7 +2729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
@@ -2031,7 +2746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
@@ -2048,7 +2763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>55</v>
       </c>
@@ -2065,7 +2780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>56</v>
       </c>
@@ -2082,7 +2797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
@@ -2099,7 +2814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>58</v>
       </c>
@@ -2116,14 +2831,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="20"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2135,24 +2850,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>86</v>
       </c>
@@ -2195,7 +2910,7 @@
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
@@ -2228,7 +2943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
@@ -2260,7 +2975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>88</v>
       </c>
@@ -2292,7 +3007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>89</v>
       </c>
@@ -2324,7 +3039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>90</v>
       </c>
@@ -2356,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>91</v>
       </c>
@@ -2388,7 +3103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>92</v>
       </c>
@@ -2420,7 +3135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
@@ -2452,7 +3167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>94</v>
       </c>
@@ -2484,7 +3199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>95</v>
       </c>
@@ -2516,7 +3231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>96</v>
       </c>
@@ -2548,7 +3263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>97</v>
       </c>
@@ -2580,7 +3295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>98</v>
       </c>
@@ -2612,7 +3327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>99</v>
       </c>
@@ -2644,7 +3359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>100</v>
       </c>
@@ -2676,7 +3391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>101</v>
       </c>
@@ -2708,7 +3423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -2740,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>102</v>
       </c>
@@ -2772,7 +3487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -2804,7 +3519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>103</v>
       </c>
@@ -2826,7 +3541,7 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -2838,7 +3553,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2848,600 +3563,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
-  <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>4</v>
-      </c>
-      <c r="D3" s="8">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8">
-        <v>6</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8">
-        <v>4</v>
-      </c>
-      <c r="J3" s="8">
-        <v>5</v>
-      </c>
-      <c r="K3" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="8">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8">
-        <v>4</v>
-      </c>
-      <c r="D4" s="8">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="H4" s="8">
-        <v>2</v>
-      </c>
-      <c r="I4" s="8">
-        <v>4</v>
-      </c>
-      <c r="J4" s="8">
-        <v>5</v>
-      </c>
-      <c r="K4" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>5</v>
-      </c>
-      <c r="E5" s="8">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="8">
-        <v>3</v>
-      </c>
-      <c r="I5" s="8">
-        <v>4</v>
-      </c>
-      <c r="J5" s="8">
-        <v>5</v>
-      </c>
-      <c r="K5" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>6</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="8">
-        <v>4</v>
-      </c>
-      <c r="I6" s="8">
-        <v>4</v>
-      </c>
-      <c r="J6" s="8">
-        <v>5</v>
-      </c>
-      <c r="K6" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="8">
-        <v>4</v>
-      </c>
-      <c r="D7" s="8">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8">
-        <v>6</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="8">
-        <v>5</v>
-      </c>
-      <c r="I7" s="8">
-        <v>4</v>
-      </c>
-      <c r="J7" s="8">
-        <v>5</v>
-      </c>
-      <c r="K7" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="8">
-        <v>4</v>
-      </c>
-      <c r="D8" s="8">
-        <v>5</v>
-      </c>
-      <c r="E8" s="8">
-        <v>6</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="8">
-        <v>6</v>
-      </c>
-      <c r="I8" s="8">
-        <v>4</v>
-      </c>
-      <c r="J8" s="8">
-        <v>5</v>
-      </c>
-      <c r="K8" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="8">
-        <v>4</v>
-      </c>
-      <c r="D9" s="8">
-        <v>5</v>
-      </c>
-      <c r="E9" s="8">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H9" s="8">
-        <v>7</v>
-      </c>
-      <c r="I9" s="8">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8">
-        <v>5</v>
-      </c>
-      <c r="K9" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" s="8">
-        <v>4</v>
-      </c>
-      <c r="D10" s="8">
-        <v>5</v>
-      </c>
-      <c r="E10" s="8">
-        <v>6</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H10" s="8">
-        <v>8</v>
-      </c>
-      <c r="I10" s="8">
-        <v>4</v>
-      </c>
-      <c r="J10" s="8">
-        <v>5</v>
-      </c>
-      <c r="K10" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="18">
-        <v>9</v>
-      </c>
-      <c r="C11" s="18">
-        <v>1</v>
-      </c>
-      <c r="D11" s="18">
-        <v>2</v>
-      </c>
-      <c r="E11" s="18">
-        <v>3</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="18">
-        <v>9</v>
-      </c>
-      <c r="I11" s="18">
-        <v>1</v>
-      </c>
-      <c r="J11" s="18">
-        <v>2</v>
-      </c>
-      <c r="K11" s="18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:18">
-      <c r="A13" s="3"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A8:G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="8">
-        <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>2</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="8">
-        <v>3</v>
-      </c>
-      <c r="C4" s="9">
-        <v>3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="8">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="8">
-        <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5</v>
-      </c>
-      <c r="E6" s="8">
-        <v>5</v>
-      </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="18">
-        <v>6</v>
-      </c>
-      <c r="C7" s="24">
-        <v>6</v>
-      </c>
-      <c r="D7" s="18">
-        <v>6</v>
-      </c>
-      <c r="E7" s="18">
-        <v>6</v>
-      </c>
-      <c r="F7" s="18">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="3"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>